<commit_message>
updates metadata with responses from Steve
</commit_message>
<xml_diff>
--- a/data-raw/metadata/daily-info-environmental-data-metadata.xlsx
+++ b/data-raw/metadata/daily-info-environmental-data-metadata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/liz/Documents/code/stanislaus-steelhead/data-raw/metadata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF365F96-B288-F14D-98A0-C78C3B1545FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CF65900-FFAC-0C47-869D-500357E55068}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17460" tabRatio="834" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -142,9 +142,6 @@
     <t>Water temperature at end of day</t>
   </si>
   <si>
-    <t>Secchi disk depth</t>
-  </si>
-  <si>
     <t>Initials of crew who did sampling</t>
   </si>
   <si>
@@ -199,13 +196,16 @@
     <t>2022-04-27</t>
   </si>
   <si>
-    <t>Flow measured at site</t>
-  </si>
-  <si>
-    <t>Time at beginning of sampling</t>
-  </si>
-  <si>
-    <t>Time at end of sampling</t>
+    <t>River flow from a gauging station</t>
+  </si>
+  <si>
+    <t>Time when the survey begins</t>
+  </si>
+  <si>
+    <t>Time when the survey ends</t>
+  </si>
+  <si>
+    <t>Secchi disk depth, measured in feet</t>
   </si>
 </sst>
 </file>
@@ -660,7 +660,7 @@
   <dimension ref="A1:AMG17"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="19.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -730,27 +730,27 @@
         <v>32</v>
       </c>
       <c r="C2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F2" s="3"/>
       <c r="G2" s="3"/>
       <c r="H2" s="3"/>
       <c r="I2" s="5"/>
       <c r="J2" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="K2" s="5"/>
       <c r="L2" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="M2" s="7" t="s">
         <v>55</v>
-      </c>
-      <c r="M2" s="7" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.2">
@@ -761,13 +761,13 @@
         <v>33</v>
       </c>
       <c r="C3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D3" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="E3" t="s">
         <v>48</v>
-      </c>
-      <c r="E3" t="s">
-        <v>49</v>
       </c>
       <c r="F3" s="3"/>
       <c r="G3" s="3"/>
@@ -786,13 +786,13 @@
         <v>34</v>
       </c>
       <c r="C4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D4" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="E4" t="s">
         <v>48</v>
-      </c>
-      <c r="E4" t="s">
-        <v>49</v>
       </c>
       <c r="F4" s="3"/>
       <c r="G4" s="3"/>
@@ -811,13 +811,13 @@
         <v>35</v>
       </c>
       <c r="C5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D5" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="E5" t="s">
         <v>48</v>
-      </c>
-      <c r="E5" t="s">
-        <v>49</v>
       </c>
       <c r="F5" s="3"/>
       <c r="G5" s="3"/>
@@ -833,16 +833,16 @@
         <v>20</v>
       </c>
       <c r="B6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C6" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D6" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="E6" t="s">
         <v>48</v>
-      </c>
-      <c r="E6" t="s">
-        <v>49</v>
       </c>
       <c r="F6" s="3"/>
       <c r="G6" s="3"/>
@@ -858,16 +858,16 @@
         <v>21</v>
       </c>
       <c r="B7" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C7" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D7" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="E7" t="s">
         <v>48</v>
-      </c>
-      <c r="E7" t="s">
-        <v>49</v>
       </c>
       <c r="F7" s="3"/>
       <c r="G7" s="3"/>
@@ -883,16 +883,16 @@
         <v>22</v>
       </c>
       <c r="B8" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C8" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D8" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="E8" t="s">
         <v>48</v>
-      </c>
-      <c r="E8" t="s">
-        <v>49</v>
       </c>
       <c r="F8" s="3"/>
       <c r="G8" s="3"/>
@@ -908,16 +908,16 @@
         <v>23</v>
       </c>
       <c r="B9" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C9" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D9" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="E9" t="s">
         <v>48</v>
-      </c>
-      <c r="E9" t="s">
-        <v>49</v>
       </c>
       <c r="F9" s="3"/>
       <c r="G9" s="3"/>
@@ -933,16 +933,16 @@
         <v>24</v>
       </c>
       <c r="B10" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C10" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D10" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="E10" t="s">
         <v>48</v>
-      </c>
-      <c r="E10" t="s">
-        <v>49</v>
       </c>
       <c r="F10" s="3"/>
       <c r="G10" s="6"/>
@@ -958,25 +958,25 @@
         <v>25</v>
       </c>
       <c r="B11" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C11" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E11" t="s">
+        <v>49</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="G11" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="H11" s="3" t="s">
         <v>50</v>
-      </c>
-      <c r="F11" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="G11" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="H11" s="3" t="s">
-        <v>51</v>
       </c>
       <c r="I11" s="5"/>
       <c r="J11" s="3"/>
@@ -993,16 +993,16 @@
         <v>26</v>
       </c>
       <c r="B12" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C12" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D12" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="E12" t="s">
         <v>48</v>
-      </c>
-      <c r="E12" t="s">
-        <v>49</v>
       </c>
       <c r="F12" s="3"/>
       <c r="G12" s="3"/>
@@ -1018,16 +1018,16 @@
         <v>27</v>
       </c>
       <c r="B13" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C13" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D13" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="E13" t="s">
         <v>48</v>
-      </c>
-      <c r="E13" t="s">
-        <v>49</v>
       </c>
       <c r="F13" s="3"/>
       <c r="G13" s="3"/>
@@ -1043,16 +1043,16 @@
         <v>28</v>
       </c>
       <c r="B14" t="s">
-        <v>38</v>
+        <v>59</v>
       </c>
       <c r="C14" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D14" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="E14" t="s">
         <v>48</v>
-      </c>
-      <c r="E14" t="s">
-        <v>49</v>
       </c>
       <c r="F14" s="3"/>
       <c r="G14" s="3"/>
@@ -1071,22 +1071,22 @@
         <v>36</v>
       </c>
       <c r="C15" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D15" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E15" t="s">
+        <v>49</v>
+      </c>
+      <c r="F15" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="G15" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="H15" s="3" t="s">
         <v>50</v>
-      </c>
-      <c r="F15" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="G15" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="H15" s="3" t="s">
-        <v>51</v>
       </c>
       <c r="I15" s="5"/>
       <c r="J15" s="3"/>
@@ -1106,22 +1106,22 @@
         <v>37</v>
       </c>
       <c r="C16" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E16" t="s">
+        <v>49</v>
+      </c>
+      <c r="F16" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="G16" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="H16" s="3" t="s">
         <v>50</v>
-      </c>
-      <c r="F16" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="G16" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="H16" s="3" t="s">
-        <v>51</v>
       </c>
       <c r="I16" s="5"/>
       <c r="J16" s="3"/>
@@ -1138,16 +1138,16 @@
         <v>31</v>
       </c>
       <c r="B17" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C17" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D17" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="E17" t="s">
         <v>48</v>
-      </c>
-      <c r="E17" t="s">
-        <v>49</v>
       </c>
       <c r="F17" s="3"/>
       <c r="G17" s="3"/>

</xml_diff>